<commit_message>
error message and index reload
</commit_message>
<xml_diff>
--- a/01-data/accuracy_export.xlsx
+++ b/01-data/accuracy_export.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8854961832061069</v>
+        <v>0.8625954198473282</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8701923076923077</v>
+        <v>0.9244935543278084</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9329896907216495</v>
+        <v>0.8297520661157025</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.900497512437811</v>
+        <v>0.8745644599303136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added First buy fx
</commit_message>
<xml_diff>
--- a/01-data/accuracy_export.xlsx
+++ b/01-data/accuracy_export.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.898854961832061</v>
+        <v>0.8998091603053435</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9153605015673981</v>
+        <v>0.9167974882260597</v>
       </c>
     </row>
     <row r="4">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9167974882260597</v>
+        <v>0.9175176747839748</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move index input tables
</commit_message>
<xml_diff>
--- a/01-data/accuracy_export.xlsx
+++ b/01-data/accuracy_export.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8624641833810889</v>
+        <v>0.9083094555873925</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9243542435424354</v>
+        <v>0.913961038961039</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8294701986754967</v>
+        <v>0.929042904290429</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8743455497382199</v>
+        <v>0.9214402618657938</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added best model excel export and se max feature =sqrt
</commit_message>
<xml_diff>
--- a/01-data/accuracy_export.xlsx
+++ b/01-data/accuracy_export.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9235912129894938</v>
+        <v>0.9083094555873925</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9331306990881459</v>
+        <v>0.913961038961039</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9446153846153846</v>
+        <v>0.929042904290429</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9388379204892966</v>
+        <v>0.9214402618657938</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor updates to default hyper parms
</commit_message>
<xml_diff>
--- a/01-data/accuracy_export.xlsx
+++ b/01-data/accuracy_export.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9083094555873925</v>
+        <v>0.897803247373448</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.913961038961039</v>
+        <v>0.9214659685863874</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.929042904290429</v>
+        <v>0.8949152542372881</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9214402618657938</v>
+        <v>0.9079965606190885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to print parms
</commit_message>
<xml_diff>
--- a/01-data/accuracy_export.xlsx
+++ b/01-data/accuracy_export.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.897803247373448</v>
+        <v>0.9083094555873925</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9214659685863874</v>
+        <v>0.913961038961039</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8949152542372881</v>
+        <v>0.929042904290429</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9079965606190885</v>
+        <v>0.9214402618657938</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding company details fetch
</commit_message>
<xml_diff>
--- a/01-data/accuracy_export.xlsx
+++ b/01-data/accuracy_export.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9083094555873925</v>
+        <v>0.8589132507149666</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.913961038961039</v>
+        <v>0.840625</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.929042904290429</v>
+        <v>0.9212328767123288</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9214402618657938</v>
+        <v>0.8790849673202614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added company to stock.html
</commit_message>
<xml_diff>
--- a/01-data/accuracy_export.xlsx
+++ b/01-data/accuracy_export.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8589132507149666</v>
+        <v>0.8446139180171592</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.840625</v>
+        <v>0.8368</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9212328767123288</v>
+        <v>0.8955479452054794</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8790849673202614</v>
+        <v>0.8651778329197684</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set hyper parms defaults llower
</commit_message>
<xml_diff>
--- a/01-data/accuracy_export.xlsx
+++ b/01-data/accuracy_export.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8586437440305635</v>
+        <v>0.8443170964660937</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.840625</v>
+        <v>0.8368</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9212328767123288</v>
+        <v>0.8955479452054794</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8790849673202614</v>
+        <v>0.8651778329197684</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving new landling page site
</commit_message>
<xml_diff>
--- a/01-data/accuracy_export.xlsx
+++ b/01-data/accuracy_export.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9016236867239733</v>
+        <v>0.8997134670487106</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9169381107491856</v>
+        <v>0.8826291079812206</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9154471544715447</v>
+        <v>0.9494949494949495</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9161920260374288</v>
+        <v>0.9148418491484185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added home page with project placeholder
</commit_message>
<xml_diff>
--- a/01-data/accuracy_export.xlsx
+++ b/01-data/accuracy_export.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8997134670487106</v>
+        <v>0.8911174785100286</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8826291079812206</v>
+        <v>0.8961038961038961</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9494949494949495</v>
+        <v>0.8927911275415896</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9148418491484185</v>
+        <v>0.8944444444444445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename Script directory and reference
</commit_message>
<xml_diff>
--- a/01-data/accuracy_export.xlsx
+++ b/01-data/accuracy_export.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8911174785100286</v>
+        <v>0.9016236867239733</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8961038961038961</v>
+        <v>0.9169381107491856</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8927911275415896</v>
+        <v>0.9154471544715447</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8944444444444445</v>
+        <v>0.9161920260374288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>